<commit_message>
Try ko lang, medyo may error e.
</commit_message>
<xml_diff>
--- a/Document/wordsentenceCOUNT.xlsx
+++ b/Document/wordsentenceCOUNT.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JUSTINC\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JUSTINC\Desktop\SumMe\Document\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="5385"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="5385" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="WORD COUNT" sheetId="1" r:id="rId1"/>
@@ -298,10 +298,10 @@
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -586,8 +586,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D70"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -599,12 +599,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
@@ -644,6 +644,9 @@
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>6</v>
+      </c>
+      <c r="B6">
+        <v>284</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -979,8 +982,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D70"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -992,12 +995,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
@@ -1037,6 +1040,9 @@
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>6</v>
+      </c>
+      <c r="B6">
+        <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Modify wordsentenceCOUNT.xlsx for ENGLISH
</commit_message>
<xml_diff>
--- a/Document/wordsentenceCOUNT.xlsx
+++ b/Document/wordsentenceCOUNT.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="5385"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="5385" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="WORD COUNT" sheetId="1" r:id="rId1"/>
@@ -592,8 +592,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D72"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView topLeftCell="A64" workbookViewId="0">
+      <selection activeCell="C72" sqref="C72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -628,7 +628,7 @@
         <v>0</v>
       </c>
       <c r="B3">
-        <v>31</v>
+        <v>331</v>
       </c>
       <c r="C3">
         <v>49</v>
@@ -641,6 +641,9 @@
       <c r="B4">
         <v>400</v>
       </c>
+      <c r="C4">
+        <v>37</v>
+      </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
@@ -649,6 +652,9 @@
       <c r="B5">
         <v>206</v>
       </c>
+      <c r="C5">
+        <v>26</v>
+      </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
@@ -657,6 +663,9 @@
       <c r="B6">
         <v>284</v>
       </c>
+      <c r="C6">
+        <v>64</v>
+      </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
@@ -665,6 +674,9 @@
       <c r="B7">
         <v>460</v>
       </c>
+      <c r="C7">
+        <v>111</v>
+      </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
@@ -673,6 +685,9 @@
       <c r="B8">
         <v>733</v>
       </c>
+      <c r="C8">
+        <v>81</v>
+      </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
@@ -681,6 +696,9 @@
       <c r="B9">
         <v>373</v>
       </c>
+      <c r="C9">
+        <v>58</v>
+      </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
@@ -689,6 +707,9 @@
       <c r="B10">
         <v>117</v>
       </c>
+      <c r="C10">
+        <v>21</v>
+      </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
@@ -697,6 +718,9 @@
       <c r="B11">
         <v>490</v>
       </c>
+      <c r="C11">
+        <v>76</v>
+      </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
@@ -710,6 +734,9 @@
       <c r="B13">
         <v>728</v>
       </c>
+      <c r="C13">
+        <v>102</v>
+      </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
@@ -718,6 +745,9 @@
       <c r="B14">
         <v>433</v>
       </c>
+      <c r="C14">
+        <v>64</v>
+      </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
@@ -726,6 +756,9 @@
       <c r="B15">
         <v>85</v>
       </c>
+      <c r="C15">
+        <v>8</v>
+      </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
@@ -734,445 +767,610 @@
       <c r="B16">
         <v>1039</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C16">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>17</v>
       </c>
       <c r="B17">
         <v>608</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C17">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>18</v>
       </c>
       <c r="B18">
         <v>326</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C18">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>19</v>
       </c>
       <c r="B19">
         <v>772</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C19">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>20</v>
       </c>
       <c r="B20">
         <v>663</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C20">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>21</v>
       </c>
       <c r="B21">
         <v>713</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C21">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>22</v>
       </c>
       <c r="B22">
         <v>684</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C22">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>23</v>
       </c>
       <c r="B23">
         <v>601</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C23">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>24</v>
       </c>
       <c r="B24">
         <v>749</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C24">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>25</v>
       </c>
       <c r="B25">
         <v>396</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C25">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>26</v>
       </c>
       <c r="B26">
         <v>631</v>
       </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C26">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>28</v>
       </c>
       <c r="B28">
         <v>239</v>
       </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C28">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>29</v>
       </c>
       <c r="B29">
         <v>321</v>
       </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C29">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>30</v>
       </c>
       <c r="B30">
         <v>525</v>
       </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C30">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>31</v>
       </c>
       <c r="B31">
         <v>526</v>
       </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C31">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>32</v>
       </c>
       <c r="B32">
         <v>431</v>
       </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C32">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>33</v>
       </c>
       <c r="B33">
         <v>819</v>
       </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C33">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>34</v>
       </c>
       <c r="B34">
         <v>264</v>
       </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C34">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>35</v>
       </c>
       <c r="B35">
         <v>363</v>
       </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C35">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>36</v>
       </c>
       <c r="B36">
         <v>153</v>
       </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C36">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>37</v>
       </c>
       <c r="B37">
         <v>324</v>
       </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C37">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>38</v>
       </c>
       <c r="B38">
         <v>209</v>
       </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C38">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>39</v>
       </c>
       <c r="B39">
         <v>823</v>
       </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C39">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>40</v>
       </c>
       <c r="B40">
         <v>97</v>
       </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C40">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>41</v>
       </c>
       <c r="B41">
         <v>587</v>
       </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C41">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>42</v>
       </c>
       <c r="B42">
         <v>652</v>
       </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C42">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>43</v>
       </c>
       <c r="B43">
         <v>271</v>
       </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C43">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>44</v>
       </c>
       <c r="B44">
         <v>413</v>
       </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C44">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>45</v>
       </c>
       <c r="B45">
         <v>758</v>
       </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C45">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>46</v>
       </c>
       <c r="B46">
         <v>414</v>
       </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C46">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>47</v>
       </c>
       <c r="B47">
         <v>579</v>
       </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C47">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>48</v>
       </c>
       <c r="B48">
         <v>233</v>
       </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C48">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>49</v>
       </c>
       <c r="B49">
         <v>365</v>
       </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C49">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>50</v>
       </c>
       <c r="B50">
         <v>492</v>
       </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C50">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>51</v>
       </c>
       <c r="B51">
         <v>922</v>
       </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C51">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>52</v>
       </c>
       <c r="B52">
         <v>667</v>
       </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C52">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>53</v>
       </c>
       <c r="B53">
         <v>411</v>
       </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C53">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>54</v>
       </c>
       <c r="B54">
         <v>403</v>
       </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C54">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>55</v>
       </c>
       <c r="B55">
         <v>770</v>
       </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C55">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>56</v>
       </c>
       <c r="B56">
         <v>476</v>
       </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C56">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>57</v>
       </c>
       <c r="B57">
         <v>372</v>
       </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C57">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>58</v>
       </c>
       <c r="B58">
         <v>527</v>
       </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C58">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>59</v>
       </c>
       <c r="B59">
         <v>662</v>
       </c>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C59">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>60</v>
       </c>
       <c r="B60">
         <v>230</v>
       </c>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C60">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>61</v>
       </c>
       <c r="B61">
         <v>343</v>
       </c>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C61">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>62</v>
       </c>
       <c r="B62">
         <v>849</v>
       </c>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C62">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>63</v>
       </c>
       <c r="B63">
         <v>145</v>
       </c>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C63">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>64</v>
       </c>
       <c r="B64">
         <v>391</v>
       </c>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C64">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>65</v>
       </c>
       <c r="B65">
         <v>564</v>
       </c>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C65">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>66</v>
       </c>
       <c r="B66">
         <v>425</v>
       </c>
-    </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C66">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>67</v>
       </c>
       <c r="B67">
         <v>285</v>
       </c>
-    </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C67">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>68</v>
       </c>
       <c r="B68">
         <v>297</v>
       </c>
-    </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C68">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>69</v>
       </c>
       <c r="B69">
         <v>467</v>
       </c>
-    </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C69">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>70</v>
       </c>
       <c r="B70">
         <v>226</v>
       </c>
-    </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C70">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>73</v>
       </c>
       <c r="B71">
         <v>744</v>
       </c>
-    </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C71">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>74</v>
       </c>
@@ -1193,8 +1391,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D72"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" topLeftCell="A60" workbookViewId="0">
+      <selection activeCell="C72" sqref="C72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1242,6 +1440,9 @@
       <c r="B4">
         <v>15</v>
       </c>
+      <c r="C4">
+        <v>6</v>
+      </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
@@ -1250,6 +1451,9 @@
       <c r="B5">
         <v>10</v>
       </c>
+      <c r="C5">
+        <v>4</v>
+      </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
@@ -1258,6 +1462,9 @@
       <c r="B6">
         <v>21</v>
       </c>
+      <c r="C6">
+        <v>8</v>
+      </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
@@ -1266,6 +1473,9 @@
       <c r="B7">
         <v>26</v>
       </c>
+      <c r="C7">
+        <v>13</v>
+      </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
@@ -1274,6 +1484,9 @@
       <c r="B8">
         <v>29</v>
       </c>
+      <c r="C8">
+        <v>11</v>
+      </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
@@ -1282,6 +1495,9 @@
       <c r="B9">
         <v>16</v>
       </c>
+      <c r="C9">
+        <v>8</v>
+      </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
@@ -1290,6 +1506,9 @@
       <c r="B10">
         <v>7</v>
       </c>
+      <c r="C10">
+        <v>3</v>
+      </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
@@ -1298,6 +1517,9 @@
       <c r="B11">
         <v>26</v>
       </c>
+      <c r="C11">
+        <v>10</v>
+      </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
@@ -1311,6 +1533,9 @@
       <c r="B13">
         <v>31</v>
       </c>
+      <c r="C13">
+        <v>12</v>
+      </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
@@ -1319,6 +1544,9 @@
       <c r="B14">
         <v>23</v>
       </c>
+      <c r="C14">
+        <v>12</v>
+      </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
@@ -1327,6 +1555,9 @@
       <c r="B15">
         <v>3</v>
       </c>
+      <c r="C15">
+        <v>1</v>
+      </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
@@ -1335,445 +1566,610 @@
       <c r="B16">
         <v>53</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C16">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>17</v>
       </c>
       <c r="B17">
         <v>25</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C17">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>18</v>
       </c>
       <c r="B18">
         <v>17</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C18">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>19</v>
       </c>
       <c r="B19">
         <v>35</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C19">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>20</v>
       </c>
       <c r="B20">
         <v>29</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C20">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>21</v>
       </c>
       <c r="B21">
         <v>43</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C21">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>22</v>
       </c>
       <c r="B22">
         <v>28</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C22">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>23</v>
       </c>
       <c r="B23">
         <v>29</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C23">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>24</v>
       </c>
       <c r="B24">
         <v>33</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C24">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>25</v>
       </c>
       <c r="B25">
         <v>14</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>26</v>
       </c>
       <c r="B26">
         <v>27</v>
       </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C26">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>28</v>
       </c>
       <c r="B28">
         <v>12</v>
       </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C28">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>29</v>
       </c>
       <c r="B29">
         <v>9</v>
       </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C29">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>30</v>
       </c>
       <c r="B30">
         <v>44</v>
       </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C30">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>31</v>
       </c>
       <c r="B31">
         <v>28</v>
       </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C31">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>32</v>
       </c>
       <c r="B32">
         <v>14</v>
       </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C32">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>33</v>
       </c>
       <c r="B33">
         <v>42</v>
       </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C33">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>34</v>
       </c>
       <c r="B34">
         <v>14</v>
       </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C34">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>35</v>
       </c>
       <c r="B35">
         <v>18</v>
       </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C35">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>36</v>
       </c>
       <c r="B36">
         <v>8</v>
       </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C36">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>37</v>
       </c>
       <c r="B37">
         <v>13</v>
       </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C37">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>38</v>
       </c>
       <c r="B38">
         <v>11</v>
       </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C38">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>39</v>
       </c>
       <c r="B39">
         <v>42</v>
       </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C39">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>40</v>
       </c>
       <c r="B40">
         <v>6</v>
       </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C40">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>41</v>
       </c>
       <c r="B41">
         <v>39</v>
       </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C41">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>42</v>
       </c>
       <c r="B42">
         <v>29</v>
       </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C42">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>43</v>
       </c>
       <c r="B43">
         <v>8</v>
       </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C43">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>44</v>
       </c>
       <c r="B44">
         <v>17</v>
       </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C44">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>45</v>
       </c>
       <c r="B45">
         <v>40</v>
       </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C45">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>46</v>
       </c>
       <c r="B46">
         <v>15</v>
       </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C46">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>47</v>
       </c>
       <c r="B47">
         <v>25</v>
       </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C47">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>48</v>
       </c>
       <c r="B48">
         <v>14</v>
       </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C48">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>49</v>
       </c>
       <c r="B49">
         <v>12</v>
       </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C49">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>50</v>
       </c>
       <c r="B50">
         <v>30</v>
       </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C50">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>51</v>
       </c>
       <c r="B51">
         <v>38</v>
       </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C51">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>52</v>
       </c>
       <c r="B52">
         <v>124</v>
       </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C52">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>53</v>
       </c>
       <c r="B53">
         <v>16</v>
       </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C53">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>54</v>
       </c>
       <c r="B54">
         <v>16</v>
       </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C54">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>55</v>
       </c>
       <c r="B55">
         <v>52</v>
       </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C55">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>56</v>
       </c>
       <c r="B56">
         <v>26</v>
       </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C56">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>57</v>
       </c>
       <c r="B57">
         <v>19</v>
       </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C57">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>58</v>
       </c>
       <c r="B58">
         <v>28</v>
       </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C58">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>59</v>
       </c>
       <c r="B59">
         <v>41</v>
       </c>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C59">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>60</v>
       </c>
       <c r="B60">
         <v>8</v>
       </c>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C60">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>61</v>
       </c>
       <c r="B61">
         <v>13</v>
       </c>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C61">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>62</v>
       </c>
       <c r="B62">
         <v>47</v>
       </c>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C62">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>63</v>
       </c>
       <c r="B63">
         <v>7</v>
       </c>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C63">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>64</v>
       </c>
       <c r="B64">
         <v>15</v>
       </c>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C64">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>65</v>
       </c>
       <c r="B65">
         <v>23</v>
       </c>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C65">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>66</v>
       </c>
       <c r="B66">
         <v>27</v>
       </c>
-    </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C66">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>67</v>
       </c>
       <c r="B67">
         <v>12</v>
       </c>
-    </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C67">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>68</v>
       </c>
       <c r="B68">
         <v>11</v>
       </c>
-    </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C68">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>69</v>
       </c>
       <c r="B69">
         <v>18</v>
       </c>
-    </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C69">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>70</v>
       </c>
       <c r="B70">
         <v>14</v>
       </c>
-    </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C70">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>73</v>
       </c>
       <c r="B71">
         <v>54</v>
       </c>
-    </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C71">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>74</v>
       </c>

</xml_diff>